<commit_message>
Review of the ORSD and typos on the ontology
</commit_message>
<xml_diff>
--- a/orsd/ORSD.xlsx
+++ b/orsd/ORSD.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24030"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4960" yWindow="1300" windowWidth="19280" windowHeight="13520"/>
+    <workbookView xWindow="4956" yWindow="1296" windowWidth="19284" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="148">
   <si>
     <t>Competency Question</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Is there any on-line documentation about the software ?</t>
   </si>
   <si>
-    <t>What is the DOI for this software (or software version) ?</t>
-  </si>
-  <si>
     <t>Is this DOI associated with a particular version ?</t>
   </si>
   <si>
@@ -183,9 +180,6 @@
   </si>
   <si>
     <t>Proposed CQs by Dani (may not be totally within the scope of OntoSoft)</t>
-  </si>
-  <si>
-    <t>Should be a date. Could use dc:issued</t>
   </si>
   <si>
     <t>What are the keywords used to describe this software?</t>
@@ -227,18 +221,6 @@
     <t>What output files does the software produce?</t>
   </si>
   <si>
-    <t>hasOutputFile, Software, File</t>
-  </si>
-  <si>
-    <t>hasInputFile, Software, File</t>
-  </si>
-  <si>
-    <t>Terms not covered by any CQ</t>
-  </si>
-  <si>
-    <t>mainly these are the categories, created for the ontology to look good. Without any motivating CQ, I would remove them</t>
-  </si>
-  <si>
     <t>What is the identifier for this person? (github, email, etc)</t>
   </si>
   <si>
@@ -263,19 +245,7 @@
     </r>
   </si>
   <si>
-    <t>I would link the software to a Benchmark; and the benchmark to the information. Benchamrs can have DOIs, versions, etc!!</t>
-  </si>
-  <si>
-    <t>hasLanguage, Software, Language</t>
-  </si>
-  <si>
-    <t>Possible misunderstanding. A language could be "English". I would call it Programming language.</t>
-  </si>
-  <si>
     <t>hasMajorContributor, Software, Person</t>
-  </si>
-  <si>
-    <t>Should be dc:contributor. Or extend dc:contributor.</t>
   </si>
   <si>
     <t>hasSalientQualities, Software, TextValue</t>
@@ -320,9 +290,6 @@
     </r>
   </si>
   <si>
-    <t>Terms that Dani thinks are not correct (see comments)</t>
-  </si>
-  <si>
     <t>Why is this not covered by hasDocumentation?</t>
   </si>
   <si>
@@ -332,49 +299,6 @@
     <t>hasCreator, Software, Person</t>
   </si>
   <si>
-    <t>Should be dc:creator. Or hasSoftwareCreator and be a subprop. What if the creator is NOT a person? (e.g., an Organization)</t>
-  </si>
-  <si>
-    <t>What is an example of the value here? Can the range be associate to a class with more semantics?</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">hasCompatibleSoftware, Software, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TextValue</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">hasBenchmarkInformation, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Software, TextValue</t>
-    </r>
-  </si>
-  <si>
-    <t>Why is the range of this property NOT Software???</t>
-  </si>
-  <si>
     <t>hasCompositionDescription, Software, Composition</t>
   </si>
   <si>
@@ -387,40 +311,13 @@
     <t>hasDocumentation, Software, Location</t>
   </si>
   <si>
-    <t>Could Location be "TextValue" as well?</t>
-  </si>
-  <si>
-    <t>should be hasDOI</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">hasDoi, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SoftwareDOI, TextValue</t>
-    </r>
-  </si>
-  <si>
     <t>hasDoiVersionId, SoftwareDOI, TextValue</t>
   </si>
   <si>
-    <t>The TextValue indirection might not be necessary here.</t>
-  </si>
-  <si>
     <t>hasFileId,  File, TextValue</t>
   </si>
   <si>
     <t>hasFileType, File, TextValue</t>
-  </si>
-  <si>
-    <t>Not clear what File Type is. Is this rdf:type? Is this the extension of the file?</t>
   </si>
   <si>
     <t>no comment. Could it be aligned to p-plan?</t>
@@ -556,56 +453,129 @@
     <t>supportsOperatingSystem, Software, OperatingSystem</t>
   </si>
   <si>
-    <t>AccessibilityProperty</t>
-  </si>
-  <si>
-    <t>ContributionProperty</t>
-  </si>
-  <si>
-    <t>ResearchProprerty</t>
-  </si>
-  <si>
-    <t>DomainKnowledgeProperty</t>
-  </si>
-  <si>
-    <t>RequirementsProperty</t>
-  </si>
-  <si>
-    <t>QualityProperty</t>
-  </si>
-  <si>
-    <t>ExecutionProperty</t>
-  </si>
-  <si>
-    <t>OtherDataProperty</t>
-  </si>
-  <si>
-    <t>OtherSoftwareProperty</t>
-  </si>
-  <si>
-    <t>PublicationProperty</t>
-  </si>
-  <si>
-    <t>SoftwareEvolutionProperty</t>
-  </si>
-  <si>
-    <t>SupportCommunityProperty</t>
-  </si>
-  <si>
-    <t>TestProperty</t>
-  </si>
-  <si>
-    <t>ComprehensionProperty</t>
-  </si>
-  <si>
     <t>domainKeywords, Software, TextValue - Similar to SoftwareTag ?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hasUniqueIdentifier</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Identifier, TextValue</t>
+    </r>
+  </si>
+  <si>
+    <t>What is the Unique identifier for this software (some repositories might have assigned it an internal one) ?</t>
+  </si>
+  <si>
+    <t>no comment. Aligned to dc:contirbutor</t>
+  </si>
+  <si>
+    <t>no comment. Aligned to dc:creator</t>
+  </si>
+  <si>
+    <t>no comment. Aligned to dc: date</t>
+  </si>
+  <si>
+    <t>Who are the adopters of this software?</t>
+  </si>
+  <si>
+    <t>hasAdopter, Software, Entity</t>
+  </si>
+  <si>
+    <t>hasBenchmarkInformation, Software, BenchmarkInformation</t>
+  </si>
+  <si>
+    <t>hasCitationLocation, Citation, Location</t>
+  </si>
+  <si>
+    <t>What is the Location of this citation? (name and URL)</t>
+  </si>
+  <si>
+    <t>hasCitationText, Citation, CitationText</t>
+  </si>
+  <si>
+    <t>What is the text associtated to this citation (i.e., how to cite this paper?)</t>
+  </si>
+  <si>
+    <t>hasCommitmentOfSupport, Software, TextEntity</t>
+  </si>
+  <si>
+    <t>not sure about the difference between this one and hasSupport</t>
+  </si>
+  <si>
+    <t>hasCompatibleSoftware, Software, SoftwareDescription</t>
+  </si>
+  <si>
+    <t>no comment. Could be Software as well (if we know)</t>
+  </si>
+  <si>
+    <t>hasEmailContact, Software, TextEntity</t>
+  </si>
+  <si>
+    <t>What is the e-mail adddress contact for this software?</t>
+  </si>
+  <si>
+    <t>GetSupport</t>
+  </si>
+  <si>
+    <t>hasExecutableLocation, Software, Location</t>
+  </si>
+  <si>
+    <t>What is the URL for the executable of this software</t>
+  </si>
+  <si>
+    <t>Execute</t>
+  </si>
+  <si>
+    <t>hasFundingSources, Software, TextEntity</t>
+  </si>
+  <si>
+    <t>Who funded this software?</t>
+  </si>
+  <si>
+    <t>hasImplementationLanguage, Software, Language</t>
+  </si>
+  <si>
+    <t>hasInput, Software, File</t>
+  </si>
+  <si>
+    <t>hasOutput, Software, File</t>
+  </si>
+  <si>
+    <t>hasInputParameter, Software, Parameter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,14 +643,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -697,6 +667,11 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -707,10 +682,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -722,11 +698,12 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="4">
+    <cellStyle name="Buena" xfId="1" builtinId="26"/>
+    <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1018,17 +995,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D73"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="63.1640625" customWidth="1"/>
+    <col min="2" max="2" width="63.109375" customWidth="1"/>
     <col min="3" max="3" width="51" customWidth="1"/>
     <col min="4" max="4" width="57.6640625" customWidth="1"/>
   </cols>
@@ -1044,7 +1021,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1055,10 +1032,10 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" t="s">
-        <v>89</v>
+        <v>58</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1069,10 +1046,10 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1083,10 +1060,10 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>72</v>
+        <v>127</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1097,24 +1074,24 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>92</v>
+        <v>134</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1125,10 +1102,10 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1139,10 +1116,10 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" t="s">
-        <v>88</v>
+        <v>76</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1153,10 +1130,10 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1167,24 +1144,24 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" t="s">
-        <v>97</v>
+        <v>80</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>16</v>
+      <c r="B11" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>98</v>
+        <v>120</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1192,13 +1169,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
-      </c>
-      <c r="D12" t="s">
-        <v>101</v>
+        <v>81</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1206,13 +1183,13 @@
         <v>5</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" t="s">
-        <v>101</v>
+        <v>82</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1220,13 +1197,13 @@
         <v>5</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D14" t="s">
-        <v>104</v>
+        <v>83</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1234,13 +1211,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>145</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1248,27 +1225,27 @@
         <v>5</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>64</v>
+        <v>147</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>106</v>
+        <v>146</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1276,13 +1253,13 @@
         <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" t="s">
-        <v>74</v>
+        <v>85</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1290,41 +1267,41 @@
         <v>3</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>108</v>
-      </c>
-      <c r="D19" t="s">
-        <v>109</v>
+        <v>144</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>118</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>86</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1332,153 +1309,153 @@
         <v>3</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>24</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" t="s">
-        <v>70</v>
+        <v>90</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="C24" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="D24" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>112</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>86</v>
+        <v>69</v>
+      </c>
+      <c r="D25" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" t="s">
-        <v>58</v>
+        <v>91</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>117</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
       <c r="D28" t="s">
-        <v>114</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="C29" t="s">
-        <v>115</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>86</v>
+        <v>92</v>
+      </c>
+      <c r="D29" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>116</v>
-      </c>
-      <c r="D31" t="s">
-        <v>119</v>
+        <v>71</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>120</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>86</v>
+        <v>95</v>
+      </c>
+      <c r="D32" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1486,13 +1463,13 @@
         <v>3</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>121</v>
-      </c>
-      <c r="D33" t="s">
-        <v>122</v>
+        <v>99</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1500,13 +1477,13 @@
         <v>3</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
       <c r="D34" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1514,13 +1491,13 @@
         <v>3</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>125</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>86</v>
+        <v>102</v>
+      </c>
+      <c r="D35" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1528,27 +1505,27 @@
         <v>3</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>83</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>82</v>
+        <v>105</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1556,13 +1533,13 @@
         <v>4</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>127</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>86</v>
+        <v>73</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1570,13 +1547,13 @@
         <v>4</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>128</v>
-      </c>
-      <c r="D39" t="s">
-        <v>85</v>
+        <v>106</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1584,255 +1561,302 @@
         <v>4</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>129</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>86</v>
+        <v>107</v>
+      </c>
+      <c r="D40" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>6</v>
       </c>
-      <c r="B42" s="8" t="s">
-        <v>42</v>
+      <c r="B42" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>131</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>54</v>
+        <v>109</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>132</v>
-      </c>
-      <c r="D43" t="s">
-        <v>133</v>
+        <v>110</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>134</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>86</v>
+        <v>111</v>
+      </c>
+      <c r="D44" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>45</v>
+        <v>3</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>137</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>138</v>
+        <v>113</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" t="s">
+        <v>116</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
         <v>3</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C46" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="B47" s="3"/>
+      <c r="B47" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>52</v>
+      <c r="B48" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="C48" t="s">
-        <v>71</v>
+        <v>126</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="9" t="s">
-        <v>55</v>
+      <c r="B49" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="C49" t="s">
-        <v>154</v>
-      </c>
-      <c r="D49" t="s">
-        <v>56</v>
+        <v>128</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>3</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>135</v>
+        <v>4</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C50" t="s">
+        <v>130</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51" t="s">
+        <v>132</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" t="s">
+        <v>119</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>138</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C53" t="s">
+        <v>136</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>141</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C54" t="s">
+        <v>139</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C55" t="s">
+        <v>142</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="B56" s="3"/>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="B57" s="3"/>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="B58" s="3"/>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="B59" s="3"/>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="B60" s="3"/>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C61" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="D54" t="s">
+      <c r="B63" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4">
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="2:4">
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="2:4">
+      <c r="D67" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4">
+      <c r="B68" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4">
+      <c r="B69" t="s">
+        <v>52</v>
+      </c>
+      <c r="C69" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4">
+      <c r="B70" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
-      <c r="B55" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="B56" t="s">
-        <v>53</v>
-      </c>
-      <c r="C56" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="B57" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="B58" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="B59" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C59" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="B60" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="B61" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="B62" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="B63" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="B64" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2">
-      <c r="B65" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2">
-      <c r="B66" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2">
-      <c r="B67" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2">
-      <c r="B68" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2">
-      <c r="B69" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2">
-      <c r="B70" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2">
-      <c r="B71" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="72" spans="2:2">
-      <c r="B72" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="73" spans="2:2">
-      <c r="B73" t="s">
-        <v>153</v>
-      </c>
+    <row r="71" spans="2:4">
+      <c r="B71" s="5"/>
+    </row>
+    <row r="72" spans="2:4">
+      <c r="B72" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1842,12 +1866,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
@@ -1860,12 +1884,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>

</xml_diff>